<commit_message>
attendence xl sheet restored to it's original file
</commit_message>
<xml_diff>
--- a/attendence.xlsx
+++ b/attendence.xlsx
@@ -640,10 +640,10 @@
   <dimension ref="A1:AD73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF11" activeCellId="1" sqref="C1:G23 AF11"/>
+      <selection pane="topLeft" activeCell="AF11" activeCellId="1" sqref="C1:E10 AF11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="4" style="2" width="7.22"/>
@@ -9278,10 +9278,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" activeCellId="0" sqref="C1:G23"/>
+      <selection pane="bottomRight" activeCell="E15" activeCellId="1" sqref="C1:E10 E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -10679,10 +10679,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" activeCellId="0" sqref="C1:G23"/>
+      <selection pane="bottomRight" activeCell="E14" activeCellId="1" sqref="C1:E10 E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -12082,10 +12082,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1:G23"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -12476,17 +12476,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1072"/>
+  <dimension ref="A1:D1072"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G23" activeCellId="0" sqref="C1:G23"/>
+      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="C1:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.01"/>
   </cols>
@@ -12497,6 +12497,7 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -13876,10 +13877,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1:G23"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -15277,10 +15278,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="C1:G23"/>
+      <selection pane="bottomRight" activeCell="D17" activeCellId="1" sqref="C1:E10 D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -16679,10 +16680,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="C1:G23 B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="C1:E10 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -18080,10 +18081,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" activeCellId="0" sqref="C1:G23"/>
+      <selection pane="bottomRight" activeCell="G17" activeCellId="1" sqref="C1:E10 G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -19483,10 +19484,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="C1:G23 B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="C1:E10 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>

</xml_diff>

<commit_message>
range in get attendence changed from 73 to 74 which allow us to take attendence of 71 people of my class
</commit_message>
<xml_diff>
--- a/attendence.xlsx
+++ b/attendence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="student_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -639,11 +639,11 @@
   </sheetPr>
   <dimension ref="A1:AD73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF11" activeCellId="1" sqref="C1:E10 AF11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D64" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF11" activeCellId="0" sqref="AF11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="4" style="2" width="7.22"/>
@@ -9273,15 +9273,15 @@
   </sheetPr>
   <dimension ref="A1:A1072"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" activeCellId="1" sqref="C1:E10 E15"/>
+      <selection pane="bottomRight" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -10679,10 +10679,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" activeCellId="1" sqref="C1:E10 E14"/>
+      <selection pane="bottomRight" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -12082,10 +12082,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1:E10"/>
+      <selection pane="bottomRight" activeCell="B73" activeCellId="0" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -12476,17 +12476,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1072"/>
+  <dimension ref="A1:E1072"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="C1:E10"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.01"/>
   </cols>
@@ -12498,6 +12498,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -13877,10 +13878,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1:E10"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -15278,10 +15279,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" activeCellId="1" sqref="C1:E10 D17"/>
+      <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -16680,10 +16681,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="C1:E10 B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -18081,10 +18082,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" activeCellId="1" sqref="C1:E10 G17"/>
+      <selection pane="bottomRight" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -19484,10 +19485,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="C1:E10 B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>

</xml_diff>

<commit_message>
make the files clean
</commit_message>
<xml_diff>
--- a/attendence.xlsx
+++ b/attendence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="student_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="159">
   <si>
     <t xml:space="preserve">S.No</t>
   </si>
@@ -504,6 +504,9 @@
   <si>
     <t xml:space="preserve">ID</t>
   </si>
+  <si>
+    <t xml:space="preserve">25-Jul-2022</t>
+  </si>
 </sst>
 </file>
 
@@ -639,11 +642,11 @@
   </sheetPr>
   <dimension ref="A1:AD73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D64" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF11" activeCellId="0" sqref="AF11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="B2:B72 H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="4" style="2" width="7.22"/>
@@ -9273,15 +9276,15 @@
   </sheetPr>
   <dimension ref="A1:A1072"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="E15" activeCellId="1" sqref="B2:B72 E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -10679,10 +10682,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2:B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -12075,17 +12078,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A72"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B73" activeCellId="0" sqref="B73"/>
+      <selection pane="bottomLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2:B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -12093,6 +12096,9 @@
     <row r="1" s="6" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>157</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12483,10 +12489,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="B2:B72 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.01"/>
   </cols>
@@ -13878,10 +13884,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="B2:B72 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -15279,10 +15285,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="1" sqref="B2:B72 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -16681,10 +16687,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="B2:B72 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -18082,10 +18088,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="G17" activeCellId="1" sqref="B2:B72 G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>
@@ -19485,10 +19491,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="B2:B72 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
   </cols>

</xml_diff>